<commit_message>
added registers to excel
</commit_message>
<xml_diff>
--- a/Atmega328p map & datasheet/Atmega328p.xlsx
+++ b/Atmega328p map & datasheet/Atmega328p.xlsx
@@ -34,7 +34,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Z-register High Byte</t>
         </r>
@@ -48,9 +47,12 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">DDC6 DDC5 DDC4 DDC3 DDC2 DDC1 DDC0</t>
+          </rPr>
+          <t xml:space="preserve">	-	DDC6 DDC5 DDC4 DDC3 DDC2 DDC1 DDC0
+To use a port as output, assign 1 to it
+DDRC |= 0B00100000;
+If a port is input, you can activate its pullup resitor
+Using PORTC</t>
         </r>
       </text>
     </comment>
@@ -62,14 +64,29 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">–	–	–	–	–	OCF2B OCF2A TOV2
+          </rPr>
+          <t xml:space="preserve">Timer Interrupt Flag Register
+–	–	–	–	–	OCF2B OCF2A TOV2
 7	6	5	4	3	      2           1        0</t>
         </r>
       </text>
     </comment>
-    <comment ref="R11" authorId="0">
+    <comment ref="R12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Output Compare Register A
+Its value gets continuously compared with TCNT0.
+If they match, OCF0A bit in TIFR0 is set
+Can be used for waveform output on OC0A pin</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +94,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">[7] I: Global Interrupt Enable.
 [6] T: Bit Copy Storage
@@ -99,7 +115,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">X-, Y- and Z-pointer registers can be set to index any register in the file</t>
         </r>
@@ -113,7 +128,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Z-register Low Byte</t>
         </r>
@@ -127,9 +141,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PINC6 PINC5 PINC4 PINC3 PINC2 PINC1 PINC0</t>
+          </rPr>
+          <t xml:space="preserve">	-	PINC6 PINC5 PINC4 PINC3 PINC2 PINC1 PINC0
+PINC gets updated with PORTC values every clock cyrcle. It is digitalRead() but for every pin on PORTC</t>
         </r>
       </text>
     </comment>
@@ -141,10 +155,24 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">–	–	ICF1	 –	–	OCF1B OCF1A TOV1
-7	6	   5	 4	3	     2           1          0</t>
+          </rPr>
+          <t xml:space="preserve">Timer Interrupt Flag Register
+–	–	ICF1		–	–	OCF1B OCF1A TOV1
+7	6	   5		4	3	     2           1          0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="S12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 (8-bit)
+Its incrementation changes based on the prescaler (found on TCCR0B).
+Compares continuously with OCR0A/B registers.</t>
         </r>
       </text>
     </comment>
@@ -156,7 +184,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Y-Register High Byte</t>
         </r>
@@ -170,9 +197,12 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PORTB7 PORTB6 PORTB5 PORTB4 PORTB3 PORTB2 PORTB1 PORTB0</t>
+          </rPr>
+          <t xml:space="preserve">PORTB7 PORTB6 PORTB5 PORTB4 PORTB3 PORTB2 PORTB1 PORTB0
+By setting a bit of PORT to 1:
+	if PORT is output, the output bit is set to HIGH.
+	if PORT is input, the internal pull-up resistor is activated
+PORTB |= 0B00100000;</t>
         </r>
       </text>
     </comment>
@@ -184,12 +214,23 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">–	–	–	–	–	OCF0B OCF0A TOV0
+          </rPr>
+          <t xml:space="preserve">Timer Interrupt Flag Register
+–	–	–	–	–	OCF0B OCF0A TOV0
 7	6	5	4	3	     2           1         0
-</t>
-        </r>
+Output Compare Flags:
+OCF0B	Sets when TimerCounter0 == OCR0B
+	Executes TimerCounter0 Compare Match Interrupt
+OCF0A	Sets when TimerCounter0 ==OCR0A
+	Executes TimerCounter0 Compare Match Interrupt
+Timer Overflow flag
+TOV0  	Sets when TimerCounter0 overflows 
+	Executes TimerCounter0 Overflow Interrupt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T12" authorId="0">
+      <text>
         <r>
           <rPr>
             <sz val="11"/>
@@ -197,10 +238,133 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">OCF0B	Becomes 1 when interrupt occurs
-OCF0A	Becomes 1 when interrupt occurs
-TOV0  	Becomes 1 when interrupt occurs
-OCR0A continuesly compares with TCNTx. When matched, the above become 1, even if the interrupt is not enabled
+          <t xml:space="preserve">Timer Counter Control Register B </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Page 109 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Force Output Compare A/B bits.
+Only active when WGM Bits are non-PWM mode.
+If Set, Compare Match is forced on Waveform Generation unit.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[7] FOC0A 
+[6] FOC0B 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+[5] –	
+[4] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM01/00, found in TCCR0A</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode ana Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[3] WGM02
+Clock Select: Control </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Prescaler
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[2] CS02
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[1] CS01 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[0] CS00
 </t>
         </r>
       </text>
@@ -213,7 +377,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Y-Register Low Byte</t>
         </r>
@@ -227,9 +390,91 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">DDB7 DDB6 DDB5 DDB4 DDB3 DDB2 DDB1 DDB0</t>
+          </rPr>
+          <t xml:space="preserve">DDB7 DDB6 DDB5 DDB4 DDB3 DDB2 DDB1 DDB0
+To use a port as output, assign 1 to it
+DDRB |= 0B00100000;
+If a port is input, you can activate its pullup resitor
+Using PORTB
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="U12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Timer Counter Control Register A </t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[Page 104 Datasheet]
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Compare Match Output A Mode
+Control the OC0A (Pin 6, PWM) output behavior.
+[7] COM0A1 
+[6] COM0A0 
+Compare Match Output B Mode
+Control the OC0B (Pin 5, PWM) output behavior.
+[5] COM0B1 
+[4] COM0B0	
+[3] –	
+[2] –	
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Combined with WGM02, found in TCCR0B</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">, these control the 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b val="true"/>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Waveform Generation Mode aka Interrupt Modes
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">[1] WGM01 
+[0] WGM00</t>
         </r>
       </text>
     </comment>
@@ -241,7 +486,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">X-Register High Byte</t>
         </r>
@@ -255,9 +499,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PINB7 PINB6 PINB5 PINB4 PINB3 PINB2 PINB1 PINB0</t>
+          </rPr>
+          <t xml:space="preserve">PINB7 PINB6 PINB5 PINB4 PINB3 PINB2 PINB1 PINB0
+PINB gets updated with PORTB values every clock cyrcle. It is digitalRead() but for every pin on PORTB</t>
         </r>
       </text>
     </comment>
@@ -269,9 +513,24 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PORTD6 PORTD5 PORTD4 PORTD3 PORTD2 PORTD1 PORTD0</t>
+          </rPr>
+          <t xml:space="preserve">PORTD6 PORTD5 PORTD4 PORTD3 PORTD2 PORTD1 PORTD0
+By setting a bit of PORT to 1:
+	if PORT is output, the output bit is set to HIGH.
+	if PORT is input, the internal pull-up resistor is activated
+PORTB |= 0B00100000;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="V11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">–	–	–	–	–	PCIF2 PCIF1 PCIF0</t>
         </r>
       </text>
     </comment>
@@ -283,7 +542,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">X-Register Low Byte
 </t>
@@ -298,9 +556,12 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">DDD7 DDD6 DDD5 DDD4 DDD3 DDD2 DDD1 DDD0</t>
+          </rPr>
+          <t xml:space="preserve">DDD7 DDD6 DDD5 DDD4 DDD3 DDD2 DDD1 DDD0
+To use a port as output, assign 1 to it
+DDRD |= 0B00100000;
+If a port is input, you can activate its pullup resitor
+Using PORTD</t>
         </r>
       </text>
     </comment>
@@ -312,9 +573,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PIND7 PIND6 PIND5 PIND4 PIND3 PIND2 PIND1 PIND0</t>
+          </rPr>
+          <t xml:space="preserve">PIND7 PIND6 PIND5 PIND4 PIND3 PIND2 PIND1 PIND0
+PIND gets updated with PORTD values every clock cyrcle. It is digitalRead() but for every pin on PORTD</t>
         </r>
       </text>
     </comment>
@@ -326,9 +587,24 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">PORTC6 PORTC5 PORTC4 PORTC3 PORTC2 PORTC1 PORTC0</t>
+          </rPr>
+          <t xml:space="preserve">	-	PORTC6 PORTC5 PORTC4 PORTC3 PORTC2 PORTC1 PORTC0
+By setting a bit of PORT to 1:
+	if PORT is output, the output bit is set to HIGH.
+	if PORT is input, the internal pull-up resistor is activated
+PORTB |= 0B00100000;</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Y13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Timer/Counter0 Output Compare Register B</t>
         </r>
       </text>
     </comment>
@@ -340,7 +616,6 @@
             <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
-            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">Initial SP value.
 Is implemented as two 8-bit registers in the I/O space [SPH/SPL].
@@ -353,7 +628,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="155">
   <si>
     <t xml:space="preserve">Flash (Program FLash memory) [32K]</t>
   </si>
@@ -559,7 +834,7 @@
     <t xml:space="preserve">PINB</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">–</t>
   </si>
   <si>
     <t xml:space="preserve">20H</t>
@@ -568,7 +843,7 @@
     <t xml:space="preserve">2FH</t>
   </si>
   <si>
-    <t xml:space="preserve">PORTD7</t>
+    <t xml:space="preserve">PORTD</t>
   </si>
   <si>
     <t xml:space="preserve">DDRD</t>
@@ -601,31 +876,73 @@
     <t xml:space="preserve">3FH</t>
   </si>
   <si>
+    <t xml:space="preserve">EECR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPIOR0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIMSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EIFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCIFR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCR0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCNT0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCR0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCCR0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GTCCR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEARH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEARL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EEDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4FH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OCR0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5FH</t>
+  </si>
+  <si>
     <t xml:space="preserve">SREG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4FH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5FH</t>
   </si>
   <si>
     <t xml:space="preserve">58H</t>
@@ -785,13 +1102,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -810,11 +1126,87 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF00A933"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -822,7 +1214,18 @@
       <color rgb="FF55308D"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -830,32 +1233,16 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -865,7 +1252,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,8 +1261,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF404040"/>
-        <bgColor rgb="FF333300"/>
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
       </patternFill>
     </fill>
     <fill>
@@ -886,8 +1297,20 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF404040"/>
+        <bgColor rgb="FF333333"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFCCCCFF"/>
+        <bgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
     <fill>
@@ -897,12 +1320,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1018,7 +1456,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1042,8 +1480,59 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="51">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1052,16 +1541,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1072,6 +1557,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1080,15 +1569,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1096,63 +1585,63 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,101 +1649,134 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
@@ -1266,7 +1788,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0563C1"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -1282,7 +1804,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -1294,11 +1816,11 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF404040"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF55308D"/>
-      <rgbColor rgb="FF404040"/>
+      <rgbColor rgb="FF333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1309,15 +1831,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>77400</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>160560</xdr:rowOff>
+      <xdr:colOff>461520</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>419400</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>167760</xdr:rowOff>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>163080</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1326,86 +1848,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17137800" y="510840"/>
-          <a:ext cx="342000" cy="708480"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:rect l="l" t="t" r="r" b="b"/>
-          <a:pathLst>
-            <a:path w="955" h="1973">
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:cubicBezTo>
-                <a:pt x="238" y="0"/>
-                <a:pt x="477" y="82"/>
-                <a:pt x="477" y="164"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="477" y="821"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="477" y="903"/>
-                <a:pt x="715" y="986"/>
-                <a:pt x="954" y="986"/>
-              </a:cubicBezTo>
-              <a:cubicBezTo>
-                <a:pt x="715" y="986"/>
-                <a:pt x="477" y="1068"/>
-                <a:pt x="477" y="1150"/>
-              </a:cubicBezTo>
-              <a:lnTo>
-                <a:pt x="477" y="1807"/>
-              </a:lnTo>
-              <a:cubicBezTo>
-                <a:pt x="477" y="1889"/>
-                <a:pt x="238" y="1972"/>
-                <a:pt x="0" y="1972"/>
-              </a:cubicBezTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="3465a4"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
-        <a:fontRef idx="minor"/>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="absolute">
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>461520</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>20880</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>29</xdr:col>
-      <xdr:colOff>163440</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1" name="CustomShape 1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="17521920" y="195840"/>
-          <a:ext cx="1864800" cy="1179000"/>
+          <a:ext cx="1864440" cy="1179000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1486,19 +1930,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>426240</xdr:colOff>
+      <xdr:colOff>425880</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CustomShape 1"/>
+        <xdr:cNvPr id="1" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17144640" y="1220400"/>
-          <a:ext cx="342000" cy="1381680"/>
+          <a:ext cx="341640" cy="1381320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1564,19 +2008,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>317520</xdr:colOff>
+      <xdr:colOff>317160</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>127440</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1"/>
+        <xdr:cNvPr id="2" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17528400" y="1893960"/>
-          <a:ext cx="1397160" cy="336600"/>
+          <a:ext cx="1396800" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1641,19 +2085,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>437760</xdr:colOff>
+      <xdr:colOff>437400</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>136080</xdr:rowOff>
+      <xdr:rowOff>135720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17156160" y="2609280"/>
-          <a:ext cx="342000" cy="3485520"/>
+          <a:ext cx="341640" cy="3485160"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1719,19 +2163,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>388440</xdr:colOff>
+      <xdr:colOff>388080</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>151920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="CustomShape 1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17540640" y="4196520"/>
-          <a:ext cx="1455840" cy="336600"/>
+          <a:ext cx="1455480" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1796,19 +2240,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
-      <xdr:colOff>449640</xdr:colOff>
+      <xdr:colOff>449280</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:rowOff>11160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="CustomShape 1"/>
+        <xdr:cNvPr id="5" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17168040" y="6102000"/>
-          <a:ext cx="342000" cy="2174400"/>
+          <a:ext cx="341640" cy="2174040"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1874,19 +2318,19 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
-      <xdr:colOff>223200</xdr:colOff>
+      <xdr:colOff>222840</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="CustomShape 1"/>
+        <xdr:cNvPr id="6" name="CustomShape 1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17588160" y="7322760"/>
-          <a:ext cx="2473560" cy="336600"/>
+          <a:ext cx="2473200" cy="336600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1935,13 +2379,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
+      <xdr:colOff>182520</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>160200</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Image 1" descr=""/>
+        <xdr:cNvPr id="7" name="Image 1" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1951,7 +2395,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11235240" y="6224400"/>
-          <a:ext cx="5392800" cy="1121400"/>
+          <a:ext cx="5392440" cy="1121040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1972,13 +2416,13 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>36</xdr:col>
-      <xdr:colOff>376560</xdr:colOff>
+      <xdr:colOff>376200</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>95400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Image 2" descr=""/>
+        <xdr:cNvPr id="8" name="Image 2" descr=""/>
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1988,7 +2432,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="19310400" y="1796400"/>
-          <a:ext cx="4578840" cy="3031200"/>
+          <a:ext cx="4578480" cy="3030840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1998,6 +2442,84 @@
         </a:ln>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>77400</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>160560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>419040</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17137800" y="510840"/>
+          <a:ext cx="341640" cy="708120"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:rect l="l" t="t" r="r" b="b"/>
+          <a:pathLst>
+            <a:path w="955" h="1973">
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:cubicBezTo>
+                <a:pt x="238" y="0"/>
+                <a:pt x="477" y="82"/>
+                <a:pt x="477" y="164"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="477" y="821"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="477" y="903"/>
+                <a:pt x="715" y="986"/>
+                <a:pt x="954" y="986"/>
+              </a:cubicBezTo>
+              <a:cubicBezTo>
+                <a:pt x="715" y="986"/>
+                <a:pt x="477" y="1068"/>
+                <a:pt x="477" y="1150"/>
+              </a:cubicBezTo>
+              <a:lnTo>
+                <a:pt x="477" y="1807"/>
+              </a:lnTo>
+              <a:cubicBezTo>
+                <a:pt x="477" y="1889"/>
+                <a:pt x="238" y="1972"/>
+                <a:pt x="0" y="1972"/>
+              </a:cubicBezTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2010,11 +2532,11 @@
   </sheetPr>
   <dimension ref="A1:AI53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T10" activeCellId="0" sqref="T10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V13" activeCellId="0" sqref="V13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="1" width="8.72"/>
@@ -2030,7 +2552,6 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="1" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="29" style="1" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="36" style="0" width="8.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2553,10 +3074,10 @@
       <c r="R10" s="28" t="s">
         <v>77</v>
       </c>
-      <c r="S10" s="29" t="s">
+      <c r="S10" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="T10" s="29" t="s">
+      <c r="T10" s="25" t="s">
         <v>79</v>
       </c>
       <c r="U10" s="25" t="s">
@@ -2574,7 +3095,7 @@
       <c r="Y10" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="Z10" s="30" t="s">
+      <c r="Z10" s="29" t="s">
         <v>80</v>
       </c>
       <c r="AA10" s="14"/>
@@ -2607,18 +3128,32 @@
       <c r="Q11" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="R11" s="31" t="s">
+      <c r="R11" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="S11" s="29"/>
-      <c r="T11" s="29"/>
-      <c r="U11" s="29"/>
-      <c r="V11" s="29"/>
-      <c r="W11" s="29"/>
-      <c r="X11" s="29"/>
-      <c r="Y11" s="32"/>
-      <c r="Z11" s="30" t="s">
+      <c r="S11" s="30" t="s">
         <v>83</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="U11" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="V11" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="W11" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="X11" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y11" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" s="29" t="s">
+        <v>87</v>
       </c>
       <c r="AA11" s="14"/>
       <c r="AB11" s="8"/>
@@ -2648,18 +3183,34 @@
       <c r="O12" s="8"/>
       <c r="P12" s="8"/>
       <c r="Q12" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="R12" s="31"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="32"/>
-      <c r="Z12" s="30" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="R12" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="S12" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="T12" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="U12" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="V12" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="W12" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="X12" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y12" s="25" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z12" s="29" t="s">
+        <v>97</v>
       </c>
       <c r="AA12" s="14"/>
       <c r="AB12" s="8"/>
@@ -2689,18 +3240,20 @@
       <c r="O13" s="8"/>
       <c r="P13" s="8"/>
       <c r="Q13" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="R13" s="31"/>
-      <c r="S13" s="29"/>
-      <c r="T13" s="29"/>
-      <c r="U13" s="29"/>
-      <c r="V13" s="29"/>
-      <c r="W13" s="29"/>
-      <c r="X13" s="29"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="30" t="s">
-        <v>87</v>
+        <v>98</v>
+      </c>
+      <c r="R13" s="24"/>
+      <c r="S13" s="25"/>
+      <c r="T13" s="25"/>
+      <c r="U13" s="25"/>
+      <c r="V13" s="25"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="25"/>
+      <c r="Y13" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z13" s="29" t="s">
+        <v>100</v>
       </c>
       <c r="AA13" s="14"/>
       <c r="AB13" s="8"/>
@@ -2730,18 +3283,18 @@
       <c r="O14" s="8"/>
       <c r="P14" s="8"/>
       <c r="Q14" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="R14" s="31"/>
-      <c r="S14" s="29"/>
-      <c r="T14" s="29"/>
-      <c r="U14" s="29"/>
-      <c r="V14" s="29"/>
-      <c r="W14" s="29"/>
-      <c r="X14" s="29"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="30" t="s">
-        <v>89</v>
+        <v>101</v>
+      </c>
+      <c r="R14" s="24"/>
+      <c r="S14" s="25"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="25"/>
+      <c r="V14" s="25"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="25"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="29" t="s">
+        <v>102</v>
       </c>
       <c r="AA14" s="14"/>
       <c r="AB14" s="8"/>
@@ -2771,18 +3324,20 @@
       <c r="O15" s="8"/>
       <c r="P15" s="8"/>
       <c r="Q15" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="R15" s="31"/>
-      <c r="S15" s="29"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="29"/>
-      <c r="X15" s="29"/>
-      <c r="Y15" s="32"/>
-      <c r="Z15" s="30" t="s">
-        <v>91</v>
+        <v>103</v>
+      </c>
+      <c r="R15" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="25"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="25"/>
+      <c r="Y15" s="35"/>
+      <c r="Z15" s="29" t="s">
+        <v>105</v>
       </c>
       <c r="AA15" s="14"/>
       <c r="AB15" s="8"/>
@@ -2812,18 +3367,18 @@
       <c r="O16" s="8"/>
       <c r="P16" s="8"/>
       <c r="Q16" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="R16" s="34"/>
-      <c r="S16" s="35"/>
-      <c r="T16" s="35"/>
-      <c r="U16" s="35"/>
-      <c r="V16" s="35"/>
-      <c r="W16" s="35"/>
-      <c r="X16" s="35"/>
-      <c r="Y16" s="36"/>
-      <c r="Z16" s="30" t="s">
-        <v>93</v>
+        <v>106</v>
+      </c>
+      <c r="R16" s="36"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="37"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="38"/>
+      <c r="Z16" s="29" t="s">
+        <v>107</v>
       </c>
       <c r="AA16" s="14"/>
       <c r="AB16" s="8"/>
@@ -2853,18 +3408,18 @@
       <c r="O17" s="8"/>
       <c r="P17" s="8"/>
       <c r="Q17" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="R17" s="34"/>
-      <c r="S17" s="35"/>
-      <c r="T17" s="35"/>
-      <c r="U17" s="35"/>
-      <c r="V17" s="35"/>
-      <c r="W17" s="35"/>
-      <c r="X17" s="35"/>
-      <c r="Y17" s="36"/>
-      <c r="Z17" s="30" t="s">
-        <v>95</v>
+        <v>108</v>
+      </c>
+      <c r="R17" s="36"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="38"/>
+      <c r="Z17" s="29" t="s">
+        <v>109</v>
       </c>
       <c r="AA17" s="14"/>
       <c r="AB17" s="8"/>
@@ -2894,18 +3449,18 @@
       <c r="O18" s="8"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="R18" s="34"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="30" t="s">
-        <v>97</v>
+        <v>110</v>
+      </c>
+      <c r="R18" s="36"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="38"/>
+      <c r="Z18" s="29" t="s">
+        <v>111</v>
       </c>
       <c r="AA18" s="14"/>
       <c r="AB18" s="8"/>
@@ -2935,18 +3490,18 @@
       <c r="O19" s="8"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="R19" s="34"/>
-      <c r="S19" s="35"/>
-      <c r="T19" s="35"/>
-      <c r="U19" s="35"/>
-      <c r="V19" s="35"/>
-      <c r="W19" s="35"/>
-      <c r="X19" s="35"/>
-      <c r="Y19" s="36"/>
-      <c r="Z19" s="30" t="s">
-        <v>99</v>
+        <v>112</v>
+      </c>
+      <c r="R19" s="36"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="29" t="s">
+        <v>113</v>
       </c>
       <c r="AA19" s="14"/>
       <c r="AB19" s="8"/>
@@ -2976,18 +3531,18 @@
       <c r="O20" s="8"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="R20" s="34"/>
-      <c r="S20" s="35"/>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
-      <c r="X20" s="35"/>
-      <c r="Y20" s="36"/>
-      <c r="Z20" s="30" t="s">
-        <v>101</v>
+        <v>114</v>
+      </c>
+      <c r="R20" s="36"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="37"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="37"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="38"/>
+      <c r="Z20" s="29" t="s">
+        <v>115</v>
       </c>
       <c r="AA20" s="14"/>
       <c r="AB20" s="8"/>
@@ -3017,18 +3572,18 @@
       <c r="O21" s="8"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="R21" s="34"/>
-      <c r="S21" s="35"/>
-      <c r="T21" s="35"/>
-      <c r="U21" s="35"/>
-      <c r="V21" s="35"/>
-      <c r="W21" s="35"/>
-      <c r="X21" s="35"/>
-      <c r="Y21" s="36"/>
-      <c r="Z21" s="30" t="s">
-        <v>103</v>
+        <v>116</v>
+      </c>
+      <c r="R21" s="36"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="37"/>
+      <c r="U21" s="37"/>
+      <c r="V21" s="37"/>
+      <c r="W21" s="37"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="38"/>
+      <c r="Z21" s="29" t="s">
+        <v>117</v>
       </c>
       <c r="AA21" s="14"/>
       <c r="AB21" s="8"/>
@@ -3042,7 +3597,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -3060,18 +3615,18 @@
       <c r="O22" s="8"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="R22" s="34"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="35"/>
-      <c r="W22" s="35"/>
-      <c r="X22" s="35"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="30" t="s">
-        <v>106</v>
+        <v>119</v>
+      </c>
+      <c r="R22" s="36"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="37"/>
+      <c r="U22" s="37"/>
+      <c r="V22" s="37"/>
+      <c r="W22" s="37"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="38"/>
+      <c r="Z22" s="29" t="s">
+        <v>120</v>
       </c>
       <c r="AA22" s="14"/>
       <c r="AB22" s="8"/>
@@ -3101,18 +3656,18 @@
       <c r="O23" s="8"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="R23" s="34"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="35"/>
-      <c r="W23" s="35"/>
-      <c r="X23" s="35"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="30" t="s">
-        <v>108</v>
+        <v>121</v>
+      </c>
+      <c r="R23" s="36"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="37"/>
+      <c r="U23" s="37"/>
+      <c r="V23" s="37"/>
+      <c r="W23" s="37"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="38"/>
+      <c r="Z23" s="29" t="s">
+        <v>122</v>
       </c>
       <c r="AA23" s="14"/>
       <c r="AB23" s="8"/>
@@ -3133,7 +3688,7 @@
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="9" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="I24" s="10"/>
       <c r="J24" s="8"/>
@@ -3144,18 +3699,18 @@
       <c r="O24" s="8"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="R24" s="34"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="35"/>
-      <c r="W24" s="35"/>
-      <c r="X24" s="35"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="30" t="s">
-        <v>111</v>
+        <v>124</v>
+      </c>
+      <c r="R24" s="36"/>
+      <c r="S24" s="37"/>
+      <c r="T24" s="37"/>
+      <c r="U24" s="37"/>
+      <c r="V24" s="37"/>
+      <c r="W24" s="37"/>
+      <c r="X24" s="37"/>
+      <c r="Y24" s="38"/>
+      <c r="Z24" s="29" t="s">
+        <v>125</v>
       </c>
       <c r="AA24" s="14"/>
       <c r="AB24" s="8"/>
@@ -3185,18 +3740,18 @@
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="R25" s="34"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="35"/>
-      <c r="W25" s="35"/>
-      <c r="X25" s="35"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="30" t="s">
-        <v>113</v>
+        <v>126</v>
+      </c>
+      <c r="R25" s="36"/>
+      <c r="S25" s="37"/>
+      <c r="T25" s="37"/>
+      <c r="U25" s="37"/>
+      <c r="V25" s="37"/>
+      <c r="W25" s="37"/>
+      <c r="X25" s="37"/>
+      <c r="Y25" s="38"/>
+      <c r="Z25" s="29" t="s">
+        <v>127</v>
       </c>
       <c r="AA25" s="14"/>
       <c r="AB25" s="8"/>
@@ -3226,18 +3781,18 @@
       <c r="O26" s="8"/>
       <c r="P26" s="8"/>
       <c r="Q26" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="R26" s="34"/>
-      <c r="S26" s="35"/>
-      <c r="T26" s="35"/>
-      <c r="U26" s="35"/>
-      <c r="V26" s="35"/>
-      <c r="W26" s="35"/>
-      <c r="X26" s="35"/>
-      <c r="Y26" s="36"/>
-      <c r="Z26" s="30" t="s">
-        <v>115</v>
+        <v>128</v>
+      </c>
+      <c r="R26" s="36"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="37"/>
+      <c r="Y26" s="38"/>
+      <c r="Z26" s="29" t="s">
+        <v>129</v>
       </c>
       <c r="AA26" s="14"/>
       <c r="AB26" s="8"/>
@@ -3267,18 +3822,18 @@
       <c r="O27" s="8"/>
       <c r="P27" s="8"/>
       <c r="Q27" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="R27" s="34"/>
-      <c r="S27" s="35"/>
-      <c r="T27" s="35"/>
-      <c r="U27" s="35"/>
-      <c r="V27" s="35"/>
-      <c r="W27" s="35"/>
-      <c r="X27" s="35"/>
-      <c r="Y27" s="36"/>
-      <c r="Z27" s="30" t="s">
-        <v>117</v>
+        <v>130</v>
+      </c>
+      <c r="R27" s="36"/>
+      <c r="S27" s="37"/>
+      <c r="T27" s="37"/>
+      <c r="U27" s="37"/>
+      <c r="V27" s="37"/>
+      <c r="W27" s="37"/>
+      <c r="X27" s="37"/>
+      <c r="Y27" s="38"/>
+      <c r="Z27" s="29" t="s">
+        <v>131</v>
       </c>
       <c r="AA27" s="14"/>
       <c r="AB27" s="8"/>
@@ -3308,18 +3863,18 @@
       <c r="O28" s="8"/>
       <c r="P28" s="8"/>
       <c r="Q28" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="R28" s="34"/>
-      <c r="S28" s="35"/>
-      <c r="T28" s="35"/>
-      <c r="U28" s="35"/>
-      <c r="V28" s="35"/>
-      <c r="W28" s="35"/>
-      <c r="X28" s="35"/>
-      <c r="Y28" s="36"/>
-      <c r="Z28" s="30" t="s">
-        <v>119</v>
+        <v>132</v>
+      </c>
+      <c r="R28" s="36"/>
+      <c r="S28" s="37"/>
+      <c r="T28" s="37"/>
+      <c r="U28" s="37"/>
+      <c r="V28" s="37"/>
+      <c r="W28" s="37"/>
+      <c r="X28" s="37"/>
+      <c r="Y28" s="38"/>
+      <c r="Z28" s="29" t="s">
+        <v>133</v>
       </c>
       <c r="AA28" s="14"/>
       <c r="AB28" s="8"/>
@@ -3349,18 +3904,18 @@
       <c r="O29" s="8"/>
       <c r="P29" s="8"/>
       <c r="Q29" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="R29" s="34"/>
-      <c r="S29" s="35"/>
-      <c r="T29" s="35"/>
-      <c r="U29" s="35"/>
-      <c r="V29" s="35"/>
-      <c r="W29" s="35"/>
-      <c r="X29" s="35"/>
-      <c r="Y29" s="36"/>
-      <c r="Z29" s="30" t="s">
-        <v>121</v>
+        <v>134</v>
+      </c>
+      <c r="R29" s="36"/>
+      <c r="S29" s="37"/>
+      <c r="T29" s="37"/>
+      <c r="U29" s="37"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
+      <c r="X29" s="37"/>
+      <c r="Y29" s="38"/>
+      <c r="Z29" s="29" t="s">
+        <v>135</v>
       </c>
       <c r="AA29" s="14"/>
       <c r="AB29" s="8"/>
@@ -3374,7 +3929,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -3392,18 +3947,18 @@
       <c r="O30" s="8"/>
       <c r="P30" s="8"/>
       <c r="Q30" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="R30" s="34"/>
-      <c r="S30" s="35"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
-      <c r="V30" s="35"/>
-      <c r="W30" s="35"/>
-      <c r="X30" s="35"/>
-      <c r="Y30" s="36"/>
-      <c r="Z30" s="30" t="s">
-        <v>124</v>
+        <v>137</v>
+      </c>
+      <c r="R30" s="36"/>
+      <c r="S30" s="37"/>
+      <c r="T30" s="37"/>
+      <c r="U30" s="37"/>
+      <c r="V30" s="37"/>
+      <c r="W30" s="37"/>
+      <c r="X30" s="37"/>
+      <c r="Y30" s="38"/>
+      <c r="Z30" s="29" t="s">
+        <v>138</v>
       </c>
       <c r="AA30" s="14"/>
       <c r="AB30" s="8"/>
@@ -3433,18 +3988,18 @@
       <c r="O31" s="8"/>
       <c r="P31" s="8"/>
       <c r="Q31" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="R31" s="34"/>
-      <c r="S31" s="35"/>
-      <c r="T31" s="35"/>
-      <c r="U31" s="35"/>
-      <c r="V31" s="35"/>
-      <c r="W31" s="35"/>
-      <c r="X31" s="35"/>
-      <c r="Y31" s="36"/>
-      <c r="Z31" s="30" t="s">
-        <v>126</v>
+        <v>139</v>
+      </c>
+      <c r="R31" s="36"/>
+      <c r="S31" s="39"/>
+      <c r="T31" s="39"/>
+      <c r="U31" s="39"/>
+      <c r="V31" s="39"/>
+      <c r="W31" s="39"/>
+      <c r="X31" s="39"/>
+      <c r="Y31" s="40"/>
+      <c r="Z31" s="29" t="s">
+        <v>140</v>
       </c>
       <c r="AA31" s="14"/>
       <c r="AB31" s="8"/>
@@ -3474,18 +4029,18 @@
       <c r="O32" s="8"/>
       <c r="P32" s="8"/>
       <c r="Q32" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="R32" s="34"/>
-      <c r="S32" s="35"/>
-      <c r="T32" s="35"/>
-      <c r="U32" s="35"/>
-      <c r="V32" s="35"/>
-      <c r="W32" s="35"/>
-      <c r="X32" s="35"/>
-      <c r="Y32" s="36"/>
-      <c r="Z32" s="30" t="s">
-        <v>128</v>
+        <v>141</v>
+      </c>
+      <c r="R32" s="36"/>
+      <c r="S32" s="39"/>
+      <c r="T32" s="39"/>
+      <c r="U32" s="39"/>
+      <c r="V32" s="39"/>
+      <c r="W32" s="39"/>
+      <c r="X32" s="39"/>
+      <c r="Y32" s="40"/>
+      <c r="Z32" s="29" t="s">
+        <v>142</v>
       </c>
       <c r="AA32" s="14"/>
       <c r="AB32" s="8"/>
@@ -3515,18 +4070,18 @@
       <c r="O33" s="8"/>
       <c r="P33" s="8"/>
       <c r="Q33" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="R33" s="34"/>
-      <c r="S33" s="35"/>
-      <c r="T33" s="35"/>
-      <c r="U33" s="35"/>
-      <c r="V33" s="35"/>
-      <c r="W33" s="35"/>
-      <c r="X33" s="35"/>
-      <c r="Y33" s="36"/>
-      <c r="Z33" s="30" t="s">
-        <v>130</v>
+        <v>143</v>
+      </c>
+      <c r="R33" s="36"/>
+      <c r="S33" s="39"/>
+      <c r="T33" s="39"/>
+      <c r="U33" s="39"/>
+      <c r="V33" s="39"/>
+      <c r="W33" s="39"/>
+      <c r="X33" s="39"/>
+      <c r="Y33" s="40"/>
+      <c r="Z33" s="29" t="s">
+        <v>144</v>
       </c>
       <c r="AA33" s="14"/>
       <c r="AB33" s="8"/>
@@ -3556,18 +4111,18 @@
       <c r="O34" s="8"/>
       <c r="P34" s="8"/>
       <c r="Q34" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="R34" s="34"/>
-      <c r="S34" s="35"/>
-      <c r="T34" s="35"/>
-      <c r="U34" s="35"/>
-      <c r="V34" s="35"/>
-      <c r="W34" s="35"/>
-      <c r="X34" s="35"/>
-      <c r="Y34" s="36"/>
-      <c r="Z34" s="30" t="s">
-        <v>132</v>
+        <v>145</v>
+      </c>
+      <c r="R34" s="36"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="29" t="s">
+        <v>146</v>
       </c>
       <c r="AA34" s="14"/>
       <c r="AB34" s="8"/>
@@ -3597,22 +4152,22 @@
       <c r="O35" s="8"/>
       <c r="P35" s="8"/>
       <c r="Q35" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="R35" s="37"/>
-      <c r="S35" s="38"/>
-      <c r="T35" s="38"/>
-      <c r="U35" s="38"/>
-      <c r="V35" s="38"/>
-      <c r="W35" s="38"/>
-      <c r="X35" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="Y35" s="39" t="s">
-        <v>135</v>
-      </c>
-      <c r="Z35" s="30" t="s">
-        <v>136</v>
+        <v>147</v>
+      </c>
+      <c r="R35" s="41"/>
+      <c r="S35" s="42"/>
+      <c r="T35" s="42"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="42"/>
+      <c r="W35" s="42"/>
+      <c r="X35" s="42" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y35" s="43" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z35" s="29" t="s">
+        <v>150</v>
       </c>
       <c r="AA35" s="14"/>
       <c r="AB35" s="8"/>
@@ -3626,122 +4181,122 @@
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P36" s="1"/>
-      <c r="Q36" s="40"/>
-      <c r="Z36" s="41"/>
+      <c r="Q36" s="44"/>
+      <c r="Z36" s="45"/>
       <c r="AA36" s="1"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P37" s="1"/>
-      <c r="Q37" s="40"/>
-      <c r="Z37" s="41"/>
+      <c r="Q37" s="44"/>
+      <c r="Z37" s="45"/>
       <c r="AA37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P38" s="1"/>
-      <c r="Q38" s="40"/>
-      <c r="Z38" s="41"/>
+      <c r="Q38" s="44"/>
+      <c r="Z38" s="45"/>
       <c r="AA38" s="3"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P39" s="1"/>
-      <c r="Q39" s="40"/>
-      <c r="Z39" s="41"/>
+      <c r="Q39" s="44"/>
+      <c r="Z39" s="45"/>
       <c r="AA39" s="3"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P40" s="1"/>
-      <c r="Q40" s="40"/>
-      <c r="Z40" s="41"/>
+      <c r="Q40" s="44"/>
+      <c r="Z40" s="45"/>
       <c r="AA40" s="3"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P41" s="1"/>
-      <c r="Q41" s="40"/>
-      <c r="Z41" s="41"/>
+      <c r="Q41" s="44"/>
+      <c r="Z41" s="45"/>
       <c r="AA41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P42" s="1"/>
-      <c r="Q42" s="40"/>
-      <c r="Z42" s="41"/>
+      <c r="Q42" s="44"/>
+      <c r="Z42" s="45"/>
       <c r="AA42" s="3"/>
     </row>
     <row r="43" customFormat="false" ht="16" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P43" s="1"/>
-      <c r="Q43" s="40"/>
-      <c r="Z43" s="41"/>
+      <c r="Q43" s="44"/>
+      <c r="Z43" s="45"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="P44" s="1"/>
-      <c r="Q44" s="40"/>
-      <c r="R44" s="42"/>
-      <c r="S44" s="43" t="s">
-        <v>137</v>
-      </c>
-      <c r="T44" s="43"/>
-      <c r="U44" s="43"/>
-      <c r="V44" s="43"/>
-      <c r="W44" s="43"/>
-      <c r="X44" s="43"/>
-      <c r="Y44" s="43"/>
-      <c r="Z44" s="43"/>
+      <c r="Q44" s="44"/>
+      <c r="R44" s="46"/>
+      <c r="S44" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="T44" s="47"/>
+      <c r="U44" s="47"/>
+      <c r="V44" s="47"/>
+      <c r="W44" s="47"/>
+      <c r="X44" s="47"/>
+      <c r="Y44" s="47"/>
+      <c r="Z44" s="47"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P45" s="1"/>
-      <c r="Q45" s="40"/>
-      <c r="R45" s="44"/>
+      <c r="Q45" s="44"/>
+      <c r="R45" s="48"/>
       <c r="S45" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="Z45" s="41"/>
+        <v>152</v>
+      </c>
+      <c r="Z45" s="45"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P46" s="1"/>
-      <c r="Q46" s="40"/>
-      <c r="R46" s="45"/>
+      <c r="Q46" s="44"/>
+      <c r="R46" s="49"/>
       <c r="S46" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="Z46" s="41"/>
+        <v>153</v>
+      </c>
+      <c r="Z46" s="45"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P47" s="1"/>
-      <c r="Q47" s="40"/>
-      <c r="R47" s="46"/>
+      <c r="Q47" s="44"/>
+      <c r="R47" s="50"/>
       <c r="S47" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Z47" s="41"/>
+        <v>154</v>
+      </c>
+      <c r="Z47" s="45"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P48" s="1"/>
-      <c r="Q48" s="40"/>
-      <c r="Z48" s="41"/>
+      <c r="Q48" s="44"/>
+      <c r="Z48" s="45"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P49" s="1"/>
-      <c r="Q49" s="40"/>
-      <c r="Z49" s="41"/>
+      <c r="Q49" s="44"/>
+      <c r="Z49" s="45"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P50" s="1"/>
-      <c r="Q50" s="40"/>
-      <c r="Z50" s="41"/>
+      <c r="Q50" s="44"/>
+      <c r="Z50" s="45"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P51" s="1"/>
-      <c r="Q51" s="40"/>
-      <c r="Z51" s="41"/>
+      <c r="Q51" s="44"/>
+      <c r="Z51" s="45"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P52" s="1"/>
-      <c r="Q52" s="40"/>
-      <c r="Z52" s="41"/>
+      <c r="Q52" s="44"/>
+      <c r="Z52" s="45"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P53" s="1"/>
-      <c r="Q53" s="40"/>
-      <c r="Z53" s="41"/>
+      <c r="Q53" s="44"/>
+      <c r="Z53" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3770,14 +4325,11 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.47"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.48046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>